<commit_message>
changed titles of projects
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adriana/Desktop/csc-110-textbook-fall2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-spring2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48129F46-5EE4-B34D-B61A-E5A40425562A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20852C96-CD2C-1E4C-82B9-1B1B5FA0CE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37020" yWindow="2460" windowWidth="27640" windowHeight="16940" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>assessment</t>
   </si>
@@ -117,6 +117,18 @@
   </si>
   <si>
     <t>Final Exam</t>
+  </si>
+  <si>
+    <t>Programming Project 7</t>
+  </si>
+  <si>
+    <t>Programming Project 8</t>
+  </si>
+  <si>
+    <t>Programming Project 9</t>
+  </si>
+  <si>
+    <t>Programming Project 10</t>
   </si>
 </sst>
 </file>
@@ -472,16 +484,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EFE6EA-9B55-F140-983F-C2D0C0E00B90}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -491,7 +504,7 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -503,7 +516,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>45163</v>
+        <v>45303</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -514,7 +527,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1">
-        <v>45167</v>
+        <v>45307</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -525,7 +538,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>45174</v>
+        <v>45314</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -536,7 +549,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>45175</v>
+        <v>45315</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -547,7 +560,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1">
-        <v>45181</v>
+        <v>45321</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -555,10 +568,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1">
-        <v>45188</v>
+        <v>45322</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -566,10 +579,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>45189</v>
+        <v>45328</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -577,10 +590,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1">
-        <v>45195</v>
+        <v>45329</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -588,10 +601,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
-        <v>45196</v>
+        <v>45335</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -599,10 +612,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1">
-        <v>45202</v>
+        <v>45336</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -610,10 +623,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1">
-        <v>45209</v>
+        <v>45342</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -621,10 +634,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1">
-        <v>45210</v>
+        <v>45343</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -632,10 +645,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1">
-        <v>45223</v>
+        <v>45349</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -643,10 +656,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1">
-        <v>45224</v>
+        <v>45350</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -654,10 +667,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1">
-        <v>45230</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -665,10 +678,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1">
-        <v>45231</v>
+        <v>45364</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -676,10 +689,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1">
-        <v>45237</v>
+        <v>45370</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -687,10 +700,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1">
-        <v>45238</v>
+        <v>45371</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -698,10 +711,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1">
-        <v>45244</v>
+        <v>45377</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -709,10 +722,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1">
-        <v>45245</v>
+        <v>45378</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -720,10 +733,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1">
-        <v>45258</v>
+        <v>45384</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -731,10 +744,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C23" s="1">
-        <v>45265</v>
+        <v>45385</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -742,10 +755,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C24" s="1">
-        <v>45266</v>
+        <v>45391</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -753,10 +766,65 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="1">
+        <v>45392</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="1">
+        <v>45398</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="C25" s="1">
-        <v>45274</v>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="1">
+        <v>45399</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="1">
+        <v>45405</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="1">
+        <v>45406</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="1">
+        <v>45415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved dates around, pushed midterm to week 6
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-spring2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FE505D-FA8C-1C47-8154-A0BBB3C3285D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCE80CB-D17B-0343-BB35-C38EE4069D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
+    <workbookView xWindow="34060" yWindow="-200" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>assessment</t>
   </si>
@@ -487,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EFE6EA-9B55-F140-983F-C2D0C0E00B90}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -593,7 +593,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1">
         <v>45329</v>
@@ -637,7 +637,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1">
         <v>45343</v>
@@ -648,10 +648,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1">
-        <v>45363</v>
+        <v>45343</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -659,10 +659,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1">
-        <v>45364</v>
+        <v>45363</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -670,10 +670,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1">
-        <v>45370</v>
+        <v>45364</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -681,10 +681,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1">
-        <v>45371</v>
+        <v>45370</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -692,7 +692,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1">
         <v>45371</v>
@@ -703,10 +703,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C19" s="1">
-        <v>45377</v>
+        <v>45371</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -714,10 +714,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C20" s="1">
-        <v>45378</v>
+        <v>45377</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -725,10 +725,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1">
-        <v>45384</v>
+        <v>45378</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -736,10 +736,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C22" s="1">
-        <v>45385</v>
+        <v>45384</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -747,10 +747,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C23" s="1">
-        <v>45391</v>
+        <v>45385</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -758,10 +758,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C24" s="1">
-        <v>45392</v>
+        <v>45391</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -769,10 +769,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1">
-        <v>45399</v>
+        <v>45392</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -780,10 +780,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1">
-        <v>45405</v>
+        <v>45399</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -791,10 +791,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C27" s="1">
-        <v>45406</v>
+        <v>45405</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -802,10 +802,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C28" s="1">
-        <v>45412</v>
+        <v>45406</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -813,10 +813,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C29" s="1">
-        <v>45413</v>
+        <v>45412</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -824,9 +824,20 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="1">
+        <v>45413</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C31" s="1">
         <v>45415</v>
       </c>
     </row>

</xml_diff>

<commit_message>
shifted projects by a week
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-spring2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA805F5-5F36-2F4D-8F4A-1BE48F2A8328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD55C5B-6FAD-E648-8550-DAA1D18D6BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33260" yWindow="-200" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>assessment</t>
   </si>
@@ -129,9 +129,6 @@
   </si>
   <si>
     <t>Programming Project 10</t>
-  </si>
-  <si>
-    <t>Programming Project 11</t>
   </si>
 </sst>
 </file>
@@ -487,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EFE6EA-9B55-F140-983F-C2D0C0E00B90}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,10 +535,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1">
-        <v>45309</v>
+        <v>45315</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -549,10 +546,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>45315</v>
+        <v>45316</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -560,10 +557,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
-        <v>45316</v>
+        <v>45322</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -571,10 +568,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1">
-        <v>45322</v>
+        <v>45323</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -582,10 +579,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>45323</v>
+        <v>45329</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -593,10 +590,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1">
-        <v>45329</v>
+        <v>45330</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -604,10 +601,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1">
-        <v>45330</v>
+        <v>45336</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -615,10 +612,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1">
-        <v>45336</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -626,10 +623,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C12" s="1">
-        <v>45337</v>
+        <v>45343</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -637,10 +634,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C13" s="1">
-        <v>45343</v>
+        <v>45344</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -648,10 +645,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1">
-        <v>45344</v>
+        <v>45364</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -659,10 +656,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1">
-        <v>45364</v>
+        <v>45365</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -670,10 +667,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1">
-        <v>45365</v>
+        <v>45372</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -681,10 +678,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -692,10 +689,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1">
-        <v>45373</v>
+        <v>45378</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -703,10 +700,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1">
-        <v>45378</v>
+        <v>45379</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -714,10 +711,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C20" s="1">
-        <v>45379</v>
+        <v>45385</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -725,10 +722,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1">
-        <v>45385</v>
+        <v>45386</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -736,10 +733,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C22" s="1">
-        <v>45386</v>
+        <v>45392</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -747,10 +744,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C23" s="1">
-        <v>45392</v>
+        <v>45393</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -758,10 +755,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C24" s="1">
-        <v>45393</v>
+        <v>45399</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -769,10 +766,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1">
-        <v>45399</v>
+        <v>45400</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -780,10 +777,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1">
-        <v>45400</v>
+        <v>45406</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -791,10 +788,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C27" s="1">
-        <v>45406</v>
+        <v>45407</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -802,10 +799,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C28" s="1">
-        <v>45407</v>
+        <v>45413</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -813,26 +810,18 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1">
-        <v>45413</v>
+        <v>45415</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="1">
-        <v>45415</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B31" s="1"/>
-      <c r="C31"/>
+      <c r="B30" s="1"/>
+      <c r="C30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
moving assignments around (added a new module)
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-spring2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD55C5B-6FAD-E648-8550-DAA1D18D6BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D71A9C1-BE31-914E-9E35-30E29D7629DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>assessment</t>
   </si>
@@ -89,15 +89,9 @@
     <t>Module 9 Programming Problems</t>
   </si>
   <si>
-    <t>Module 10 Programming Problems</t>
-  </si>
-  <si>
     <t>Module 11 Programming Problems</t>
   </si>
   <si>
-    <t>Module 12 Programming Problems</t>
-  </si>
-  <si>
     <t>Programming Project 5</t>
   </si>
   <si>
@@ -129,6 +123,9 @@
   </si>
   <si>
     <t>Programming Project 10</t>
+  </si>
+  <si>
+    <t>Module 14 Programming Problems</t>
   </si>
 </sst>
 </file>
@@ -487,7 +484,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -601,7 +598,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1">
         <v>45336</v>
@@ -656,7 +653,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1">
         <v>45365</v>
@@ -678,7 +675,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1">
         <v>45373</v>
@@ -689,7 +686,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1">
         <v>45378</v>
@@ -722,7 +719,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" s="1">
         <v>45386</v>
@@ -733,7 +730,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1">
         <v>45392</v>
@@ -744,7 +741,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1">
         <v>45393</v>
@@ -766,7 +763,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25" s="1">
         <v>45400</v>
@@ -777,7 +774,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C26" s="1">
         <v>45406</v>
@@ -788,7 +785,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C27" s="1">
         <v>45407</v>
@@ -799,7 +796,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C28" s="1">
         <v>45413</v>
@@ -810,7 +807,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C29" s="1">
         <v>45415</v>

</xml_diff>

<commit_message>
shifted projects (added new project 4)
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-spring2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60B0538-DC79-424E-9C08-90738F8D712A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF7CA6D-0578-DE4A-8E64-CB7CE728A5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>assessment</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Module 14 Programming Problems</t>
+  </si>
+  <si>
+    <t>Programming Project 11</t>
   </si>
 </sst>
 </file>
@@ -481,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EFE6EA-9B55-F140-983F-C2D0C0E00B90}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,10 +623,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1">
-        <v>45343</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -631,10 +634,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1">
-        <v>45344</v>
+        <v>45343</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -642,10 +645,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1">
-        <v>45364</v>
+        <v>45344</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -653,10 +656,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1">
-        <v>45365</v>
+        <v>45364</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -664,10 +667,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1">
-        <v>45372</v>
+        <v>45365</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -675,10 +678,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1">
-        <v>45373</v>
+        <v>45372</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -686,10 +689,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1">
-        <v>45378</v>
+        <v>45373</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -697,10 +700,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C19" s="1">
-        <v>45379</v>
+        <v>45378</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -708,10 +711,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="1">
-        <v>45385</v>
+        <v>45379</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -719,10 +722,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C21" s="1">
-        <v>45386</v>
+        <v>45385</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -730,10 +733,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C22" s="1">
-        <v>45392</v>
+        <v>45386</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -741,10 +744,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C23" s="1">
-        <v>45393</v>
+        <v>45392</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -752,10 +755,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C24" s="1">
-        <v>45399</v>
+        <v>45393</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -763,10 +766,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C25" s="1">
-        <v>45400</v>
+        <v>45399</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -774,10 +777,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C26" s="1">
-        <v>45406</v>
+        <v>45400</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -785,10 +788,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C27" s="1">
-        <v>45407</v>
+        <v>45406</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -796,10 +799,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C28" s="1">
-        <v>45413</v>
+        <v>45407</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -807,15 +810,26 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="1">
+        <v>45413</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C30" s="1">
         <v>45415</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B30" s="1"/>
-      <c r="C30"/>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B31" s="1"/>
+      <c r="C31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adjusted dates, added dates for quizzes
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/picoral/Documents/csc-110-spring2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF7CA6D-0578-DE4A-8E64-CB7CE728A5E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC01B92-157D-B043-8F69-AAE056F82BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
+    <workbookView xWindow="37300" yWindow="860" windowWidth="30240" windowHeight="18880" xr2:uid="{7D31D848-01AB-0F4E-BA11-99DA0071AD25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>assessment</t>
   </si>
@@ -129,6 +129,48 @@
   </si>
   <si>
     <t>Programming Project 11</t>
+  </si>
+  <si>
+    <t>Quiz 01</t>
+  </si>
+  <si>
+    <t>Quiz 02</t>
+  </si>
+  <si>
+    <t>Quiz 03</t>
+  </si>
+  <si>
+    <t>Quiz 04</t>
+  </si>
+  <si>
+    <t>Quiz 05</t>
+  </si>
+  <si>
+    <t>Quiz 06</t>
+  </si>
+  <si>
+    <t>Quiz 07</t>
+  </si>
+  <si>
+    <t>Quiz 08</t>
+  </si>
+  <si>
+    <t>Quiz 10</t>
+  </si>
+  <si>
+    <t>Quiz 09</t>
+  </si>
+  <si>
+    <t>Quiz 11</t>
+  </si>
+  <si>
+    <t>Quiz 12</t>
+  </si>
+  <si>
+    <t>Module 10 Programming Problems</t>
+  </si>
+  <si>
+    <t>Module 12 Programming Problems</t>
   </si>
 </sst>
 </file>
@@ -484,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EFE6EA-9B55-F140-983F-C2D0C0E00B90}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,10 +555,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1">
-        <v>45303</v>
+        <v>45301</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -524,10 +566,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>45308</v>
+        <v>45303</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -535,10 +577,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1">
-        <v>45315</v>
+        <v>45308</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -546,10 +588,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>45316</v>
+        <v>45308</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -557,10 +599,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1">
-        <v>45322</v>
+        <v>45315</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -568,10 +610,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C7" s="1">
-        <v>45323</v>
+        <v>45315</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -579,10 +621,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1">
-        <v>45329</v>
+        <v>45316</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -590,10 +632,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C9" s="1">
-        <v>45330</v>
+        <v>45322</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -601,10 +643,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1">
-        <v>45336</v>
+        <v>45322</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -612,10 +654,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1">
-        <v>45337</v>
+        <v>45323</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -623,10 +665,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1">
-        <v>45338</v>
+        <v>45329</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -634,10 +676,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1">
-        <v>45343</v>
+        <v>45329</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -645,10 +687,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1">
-        <v>45344</v>
+        <v>45330</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -656,10 +698,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1">
-        <v>45364</v>
+        <v>45336</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -667,10 +709,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1">
-        <v>45365</v>
+        <v>45337</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -678,10 +720,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1">
-        <v>45372</v>
+        <v>45338</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -689,10 +731,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1">
-        <v>45373</v>
+        <v>45343</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -700,10 +742,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C19" s="1">
-        <v>45378</v>
+        <v>45343</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -711,10 +753,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1">
-        <v>45379</v>
+        <v>45344</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -722,10 +764,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C21" s="1">
-        <v>45385</v>
+        <v>45364</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -733,10 +775,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C22" s="1">
-        <v>45386</v>
+        <v>45364</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -744,10 +786,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C23" s="1">
-        <v>45392</v>
+        <v>45365</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -755,10 +797,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C24" s="1">
-        <v>45393</v>
+        <v>45371</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -766,10 +808,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C25" s="1">
-        <v>45399</v>
+        <v>45371</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -777,10 +819,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1">
-        <v>45400</v>
+        <v>45372</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -788,10 +830,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="1">
-        <v>45406</v>
+        <v>45378</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -799,10 +841,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C28" s="1">
-        <v>45407</v>
+        <v>45379</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -810,10 +852,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C29" s="1">
-        <v>45413</v>
+        <v>45385</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -821,15 +863,158 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="1">
+        <v>45385</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="1">
+        <v>45386</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="1">
+        <v>45392</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="1">
+        <v>45392</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="1">
+        <v>45393</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="1">
+        <v>45399</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="1">
+        <v>45399</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="1">
+        <v>45400</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="1">
+        <v>45406</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="1">
+        <v>45407</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="1">
+        <v>45413</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" s="1">
+        <v>45413</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="1">
+        <v>45413</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C43" s="1">
         <v>45415</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B31" s="1"/>
-      <c r="C31"/>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B44" s="1"/>
+      <c r="C44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
remove final exam date
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinchen/Documents/GitRepo/websites/csc110-fall2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67479B7-E768-824B-82CB-48C667D97CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF67D90-C588-5D4E-BA5A-20D650948495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17800" yWindow="4320" windowWidth="22480" windowHeight="24480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -224,11 +224,18 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -286,15 +293,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -513,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1248,10 +1256,8 @@
       <c r="B52" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="2">
-        <v>45639</v>
-      </c>
-      <c r="D52" s="5" t="s">
+      <c r="C52" s="2"/>
+      <c r="D52" s="9" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update final exam date
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinchen/Documents/GitRepo/websites/csc110-fall2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF67D90-C588-5D4E-BA5A-20D650948495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB73E96-6B94-CE47-8772-C407DEF98B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17800" yWindow="4320" windowWidth="22480" windowHeight="24480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15920" yWindow="500" windowWidth="22480" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -522,7 +522,7 @@
   <dimension ref="A1:F1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1256,7 +1256,9 @@
       <c r="B52" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="2"/>
+      <c r="C52" s="2">
+        <v>45639</v>
+      </c>
       <c r="D52" s="9" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
add final exam location
</commit_message>
<xml_diff>
--- a/assessment_schedule.xlsx
+++ b/assessment_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinchen/Documents/GitRepo/websites/csc110-spring2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2FB4A9-72E2-7348-B4F5-E83A6F9815DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67756FE4-6780-9C42-B66D-F9F52E225781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21700" yWindow="7420" windowWidth="22480" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15920" yWindow="2720" windowWidth="22480" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -213,13 +213,13 @@
     <t>Quiz 12</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>Final Exam 2pm Section</t>
   </si>
   <si>
     <t>Final Exam 1pm Section</t>
+  </si>
+  <si>
+    <t>1pm GITT 129B</t>
   </si>
 </sst>
 </file>
@@ -229,11 +229,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -326,17 +333,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -557,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1306,13 +1314,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C53" s="9">
         <v>45786</v>
       </c>
-      <c r="D53" s="10" t="s">
-        <v>57</v>
+      <c r="D53" s="13" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1320,13 +1328,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C54" s="9">
         <v>45789</v>
       </c>
-      <c r="D54" s="10" t="s">
-        <v>57</v>
+      <c r="D54" s="13" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>